<commit_message>
posner changed: remain rt
</commit_message>
<xml_diff>
--- a/tableResource/go_nogo.xlsx
+++ b/tableResource/go_nogo.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView windowHeight="15260"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
-    <sheet r:id="rId2" sheetId="2" name="Sheet2"/>
-    <sheet r:id="rId3" sheetId="3" name="Sheet3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -45,38 +45,380 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="宋体"/>
-      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -88,33 +430,315 @@
       <left/>
       <right/>
       <top/>
-      <bottom/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+  <cellStyles count="49">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
+    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
+    <cellStyle name="输入" xfId="4" builtinId="20"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
+    <cellStyle name="货币" xfId="7" builtinId="4"/>
+    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
+    <cellStyle name="百分比" xfId="9" builtinId="5"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
+    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
+    <cellStyle name="计算" xfId="15" builtinId="22"/>
+    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
+    <cellStyle name="适中" xfId="17" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
+    <cellStyle name="好" xfId="19" builtinId="26"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="差" xfId="22" builtinId="27"/>
+    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
+    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
+    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
+    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
+    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
+    <cellStyle name="标题" xfId="33" builtinId="15"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
+    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="注释" xfId="37" builtinId="10"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
+    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8"/>
+    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
+    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
+    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -125,10 +749,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -166,71 +790,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -258,7 +882,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -281,11 +905,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -294,13 +918,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -310,7 +934,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -319,7 +943,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -328,7 +952,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -336,10 +960,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -399,128 +1023,136 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" style="3" width="47.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="47.5769230769231" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1442307692308" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="1" t="s">
+    <row r="1" ht="19.5" customHeight="1" spans="1:2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="21">
-      <c r="A2" s="1" t="s">
+    <row r="2" ht="21" customHeight="1" spans="1:2">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="21">
-      <c r="A3" s="1" t="s">
+    <row r="3" ht="21" customHeight="1" spans="1:2">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="21">
-      <c r="A4" s="1" t="s">
+    <row r="4" ht="21" customHeight="1" spans="1:2">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="21">
-      <c r="A5" s="1" t="s">
+    <row r="5" ht="21" customHeight="1" spans="1:2">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="21">
-      <c r="A6" s="1" t="s">
+    <row r="6" ht="21" customHeight="1" spans="1:2">
+      <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="21">
-      <c r="A7" s="1" t="s">
+    <row r="7" ht="21" customHeight="1" spans="1:2">
+      <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="21">
-      <c r="A8" s="1" t="s">
+    <row r="8" ht="21" customHeight="1" spans="1:2">
+      <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="21">
-      <c r="A9" s="1" t="s">
+    <row r="9" ht="21" customHeight="1" spans="1:2">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>